<commit_message>
[VERSION]: Ethics first submission, functioning generator. TODO:
- Decide on the precise languages (too many concepts in these ones)
- Prepare and record the video material
- Finish the instrument
- Dry-run the analysis with fake data.
</commit_message>
<xml_diff>
--- a/Material/Config/config.xlsx
+++ b/Material/Config/config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\0. ProtonDrive\Other computers\DESKTOP-PR117J6\Academic\Projects\2022 - RL Generation\iRL - Experiment with Humans\Material\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dropbox\Private\Others\Academic\Projects\2022 - RL Generation\iRL - Experiment with Humans\Material\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{345B8847-51D1-4D6A-BCC4-598C8E81E44D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5509146-C882-4C8C-A623-7E687714AFAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13667" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
@@ -20,9 +20,9 @@
     <sheet name="Config" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="iRL">Concepts!$A$2:$E$17</definedName>
+    <definedName name="iRL">Concepts!$A$2:$G$17</definedName>
     <definedName name="iRLIDs">Concepts!$A$2:$A$17</definedName>
-    <definedName name="iRLs">Concepts!$A$18:$E$28</definedName>
+    <definedName name="iRLs">Concepts!$A$18:$G$28</definedName>
     <definedName name="iRLsIDs">Concepts!$A$18:$A$28</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="128">
   <si>
     <t>iRL</t>
   </si>
@@ -309,9 +309,6 @@
     <t>overlap</t>
   </si>
   <si>
-    <t>relecance</t>
-  </si>
-  <si>
     <t>completeness</t>
   </si>
   <si>
@@ -400,6 +397,39 @@
   </si>
   <si>
     <t>negatively contributes to</t>
+  </si>
+  <si>
+    <t>examples</t>
+  </si>
+  <si>
+    <t>(Actor, Effect (indirect), contributes-to, etc.)</t>
+  </si>
+  <si>
+    <t>urlAll</t>
+  </si>
+  <si>
+    <t>http://www.yorku.ca/liaskos/Projects/2022-Vocabularies/gmo.htm</t>
+  </si>
+  <si>
+    <t>http://www.yorku.ca/liaskos/Projects/2022-Vocabularies/gme.htm</t>
+  </si>
+  <si>
+    <t>relevance</t>
+  </si>
+  <si>
+    <t>definition</t>
+  </si>
+  <si>
+    <t>An active, autonomous entity that holds beliefs and aims at achieving goals.</t>
+  </si>
+  <si>
+    <t>A state of affairs that an actor wants to achieve.</t>
+  </si>
+  <si>
+    <t>trainingExample</t>
+  </si>
+  <si>
+    <t>caseTitle</t>
   </si>
 </sst>
 </file>
@@ -754,22 +784,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="92.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="92.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="38.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -792,19 +822,19 @@
         <v>26</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>64</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -841,7 +871,7 @@
         <v>Actor</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -878,7 +908,7 @@
         <v>Goal</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -915,7 +945,7 @@
         <v>Task</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -952,7 +982,7 @@
         <v>Task</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -989,7 +1019,7 @@
         <v>Effect</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1026,7 +1056,7 @@
         <v>Effect</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -1063,7 +1093,7 @@
         <v>Effect</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -1100,7 +1130,7 @@
         <v>Effect</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -1137,7 +1167,7 @@
         <v>Effect</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1174,7 +1204,7 @@
         <v>Effect (previous value)</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1211,7 +1241,7 @@
         <v>Quality</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -1248,7 +1278,7 @@
         <v>Quality</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -1285,7 +1315,7 @@
         <v>Quality</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1322,7 +1352,7 @@
         <v>Quality (previous value)</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -1359,7 +1389,7 @@
         <v>is-or-child-of</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -1396,7 +1426,7 @@
         <v>is-or-child-of</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -1433,7 +1463,7 @@
         <v>may-or-may-not-bring-about</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -1470,7 +1500,7 @@
         <v>may-or-may-not-bring-about</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -1507,7 +1537,7 @@
         <v>may-or-may-not-bring-about</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -1544,7 +1574,7 @@
         <v>may-or-may-not-bring-about</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -1581,7 +1611,7 @@
         <v>affects</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -1618,7 +1648,7 @@
         <v>affects</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1655,7 +1685,7 @@
         <v>affects</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -1692,7 +1722,7 @@
         <v>affects</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -1729,7 +1759,7 @@
         <v>affects</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -1766,7 +1796,7 @@
         <v>affects</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -1803,7 +1833,7 @@
         <v>affects</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -1840,7 +1870,7 @@
         <v>affects</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1877,7 +1907,7 @@
         <v>affects</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1921,38 +1951,46 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55A67578-F426-48F2-87A8-25344D20072D}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="38.85546875" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" customWidth="1"/>
+    <col min="2" max="2" width="38.88671875" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" customWidth="1"/>
+    <col min="5" max="5" width="61" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="61" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>110</v>
-      </c>
       <c r="E1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1966,10 +2004,17 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F2" t="str">
+        <f>"TRAINING EXAMPLE Definition -" &amp; B2</f>
+        <v>TRAINING EXAMPLE Definition -Actor</v>
+      </c>
+      <c r="G2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1983,10 +2028,17 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
+        <v>125</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F28" si="0">"TRAINING EXAMPLE Definition -" &amp; B3</f>
+        <v>TRAINING EXAMPLE Definition -Goal</v>
+      </c>
+      <c r="G3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1999,11 +2051,19 @@
       <c r="D4">
         <v>1</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="str">
+        <f>"TODO Definition -" &amp; B4</f>
+        <v>TODO Definition -Task</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>TRAINING EXAMPLE Definition -Task</v>
+      </c>
+      <c r="G4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>68</v>
       </c>
@@ -2016,11 +2076,19 @@
       <c r="D5">
         <v>1</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="str">
+        <f t="shared" ref="E5:E17" si="1">"TODO Definition -" &amp; B5</f>
+        <v>TODO Definition -Effect (task satisfying)</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>TRAINING EXAMPLE Definition -Effect (task satisfying)</v>
+      </c>
+      <c r="G5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>69</v>
       </c>
@@ -2033,11 +2101,19 @@
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" t="str">
+        <f t="shared" si="1"/>
+        <v>TODO Definition -Effect (task non-satisfying)</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>TRAINING EXAMPLE Definition -Effect (task non-satisfying)</v>
+      </c>
+      <c r="G6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -2050,11 +2126,19 @@
       <c r="D7">
         <v>1</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" t="str">
+        <f t="shared" si="1"/>
+        <v>TODO Definition -Effect (previous value)</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>TRAINING EXAMPLE Definition -Effect (previous value)</v>
+      </c>
+      <c r="G7" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>65</v>
       </c>
@@ -2067,11 +2151,19 @@
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" t="str">
+        <f t="shared" si="1"/>
+        <v>TODO Definition -Effect (indirect)</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>TRAINING EXAMPLE Definition -Effect (indirect)</v>
+      </c>
+      <c r="G8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -2084,11 +2176,19 @@
       <c r="D9">
         <v>1</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" t="str">
+        <f t="shared" si="1"/>
+        <v>TODO Definition -Quality</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>TRAINING EXAMPLE Definition -Quality</v>
+      </c>
+      <c r="G9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -2101,11 +2201,19 @@
       <c r="D10">
         <v>1</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" t="str">
+        <f t="shared" si="1"/>
+        <v>TODO Definition -Quality (previous value)</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>TRAINING EXAMPLE Definition -Quality (previous value)</v>
+      </c>
+      <c r="G10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -2118,11 +2226,19 @@
       <c r="D11">
         <v>2</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" t="str">
+        <f t="shared" si="1"/>
+        <v>TODO Definition -is-and-child-of</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>TRAINING EXAMPLE Definition -is-and-child-of</v>
+      </c>
+      <c r="G11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -2135,11 +2251,19 @@
       <c r="D12">
         <v>2</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" t="str">
+        <f t="shared" si="1"/>
+        <v>TODO Definition -is-or-child-of</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>TRAINING EXAMPLE Definition -is-or-child-of</v>
+      </c>
+      <c r="G12" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>66</v>
       </c>
@@ -2152,11 +2276,19 @@
       <c r="D13">
         <v>2</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" t="str">
+        <f t="shared" si="1"/>
+        <v>TODO Definition -affects</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>TRAINING EXAMPLE Definition -affects</v>
+      </c>
+      <c r="G13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>67</v>
       </c>
@@ -2169,16 +2301,24 @@
       <c r="D14">
         <v>2</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" t="str">
+        <f t="shared" si="1"/>
+        <v>TODO Definition -may-or-may-not-bring-about</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>TRAINING EXAMPLE Definition -may-or-may-not-bring-about</v>
+      </c>
+      <c r="G14" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
@@ -2186,16 +2326,24 @@
       <c r="D15">
         <v>2</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" t="str">
+        <f t="shared" si="1"/>
+        <v>TODO Definition -contributes to (positively or negatively)</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>TRAINING EXAMPLE Definition -contributes to (positively or negatively)</v>
+      </c>
+      <c r="G15" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>73</v>
       </c>
       <c r="B16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C16" t="s">
         <v>9</v>
@@ -2203,16 +2351,24 @@
       <c r="D16">
         <v>2</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" t="str">
+        <f t="shared" si="1"/>
+        <v>TODO Definition -positively contributes to</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
+        <v>TRAINING EXAMPLE Definition -positively contributes to</v>
+      </c>
+      <c r="G16" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>74</v>
       </c>
       <c r="B17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C17" t="s">
         <v>9</v>
@@ -2220,11 +2376,19 @@
       <c r="D17">
         <v>2</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" t="str">
+        <f t="shared" si="1"/>
+        <v>TODO Definition -negatively contributes to</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="0"/>
+        <v>TRAINING EXAMPLE Definition -negatively contributes to</v>
+      </c>
+      <c r="G17" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -2238,10 +2402,17 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
+        <v>124</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="0"/>
+        <v>TRAINING EXAMPLE Definition -Actor</v>
+      </c>
+      <c r="G18" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -2255,10 +2426,17 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
+        <v>125</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="0"/>
+        <v>TRAINING EXAMPLE Definition -Goal</v>
+      </c>
+      <c r="G19" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -2271,11 +2449,19 @@
       <c r="D20">
         <v>1</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" t="str">
+        <f>"TODO Definition -" &amp; B20</f>
+        <v>TODO Definition -Task</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="0"/>
+        <v>TRAINING EXAMPLE Definition -Task</v>
+      </c>
+      <c r="G20" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -2288,11 +2474,19 @@
       <c r="D21">
         <v>1</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" t="str">
+        <f t="shared" ref="E21:E28" si="2">"TODO Definition -" &amp; B21</f>
+        <v>TODO Definition -Effect</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="0"/>
+        <v>TRAINING EXAMPLE Definition -Effect</v>
+      </c>
+      <c r="G21" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -2305,11 +2499,19 @@
       <c r="D22">
         <v>1</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" t="str">
+        <f t="shared" si="2"/>
+        <v>TODO Definition -Effect (previous value)</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="0"/>
+        <v>TRAINING EXAMPLE Definition -Effect (previous value)</v>
+      </c>
+      <c r="G22" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -2322,11 +2524,19 @@
       <c r="D23">
         <v>1</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" t="str">
+        <f t="shared" si="2"/>
+        <v>TODO Definition -Quality</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="0"/>
+        <v>TRAINING EXAMPLE Definition -Quality</v>
+      </c>
+      <c r="G23" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -2339,11 +2549,19 @@
       <c r="D24">
         <v>1</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" t="str">
+        <f t="shared" si="2"/>
+        <v>TODO Definition -Quality (previous value)</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="0"/>
+        <v>TRAINING EXAMPLE Definition -Quality (previous value)</v>
+      </c>
+      <c r="G24" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -2356,11 +2574,19 @@
       <c r="D25">
         <v>2</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" t="str">
+        <f t="shared" si="2"/>
+        <v>TODO Definition -is-and-child-of</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="0"/>
+        <v>TRAINING EXAMPLE Definition -is-and-child-of</v>
+      </c>
+      <c r="G25" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -2373,11 +2599,19 @@
       <c r="D26">
         <v>2</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" t="str">
+        <f t="shared" si="2"/>
+        <v>TODO Definition -is-or-child-of</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="0"/>
+        <v>TRAINING EXAMPLE Definition -is-or-child-of</v>
+      </c>
+      <c r="G26" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>66</v>
       </c>
@@ -2390,11 +2624,19 @@
       <c r="D27">
         <v>2</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" t="str">
+        <f t="shared" si="2"/>
+        <v>TODO Definition -affects</v>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" si="0"/>
+        <v>TRAINING EXAMPLE Definition -affects</v>
+      </c>
+      <c r="G27" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>67</v>
       </c>
@@ -2407,7 +2649,15 @@
       <c r="D28">
         <v>2</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" t="str">
+        <f t="shared" si="2"/>
+        <v>TODO Definition -may-or-may-not-bring-about</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" si="0"/>
+        <v>TRAINING EXAMPLE Definition -may-or-may-not-bring-about</v>
+      </c>
+      <c r="G28" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2419,22 +2669,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2213172F-6AC1-42CA-8EAF-DBEE6814A5DB}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="72" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="75.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.6640625" customWidth="1"/>
+    <col min="5" max="5" width="66" customWidth="1"/>
+    <col min="6" max="6" width="14.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>75</v>
       </c>
@@ -2442,33 +2693,45 @@
         <v>76</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>77</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" t="s">
         <v>78</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>79</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>63</v>
       </c>
@@ -2476,73 +2739,87 @@
         <v>77</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>83</v>
+      </c>
+      <c r="G3" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" location="concepts" xr:uid="{645C2665-383D-484E-9957-CE3D12BF6C43}"/>
-    <hyperlink ref="D3" r:id="rId2" location="relationships" xr:uid="{BA3666BF-2274-4326-88B8-21AF91870A99}"/>
+    <hyperlink ref="D3" r:id="rId1" location="concepts" xr:uid="{645C2665-383D-484E-9957-CE3D12BF6C43}"/>
+    <hyperlink ref="E3" r:id="rId2" location="relationships" xr:uid="{BA3666BF-2274-4326-88B8-21AF91870A99}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{3CE29231-E3FA-45A8-AFE3-276D74CD3008}"/>
+    <hyperlink ref="C3" r:id="rId4" xr:uid="{BE7ADA23-5AED-4259-8874-ACDC0712E9D6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D77FB8ED-296C-4040-BCEE-A5690B45B944}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="128.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="69.140625" customWidth="1"/>
-    <col min="5" max="5" width="66.7109375" customWidth="1"/>
+    <col min="3" max="3" width="128.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="69.109375" customWidth="1"/>
+    <col min="6" max="6" width="66.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>21</v>
       </c>
       <c r="B1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="3" customFormat="1" ht="154.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="D2" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" s="3" customFormat="1" ht="154.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>104</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -2555,24 +2832,24 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" t="s">
         <v>92</v>
       </c>
-      <c r="B1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>85</v>
       </c>
@@ -2580,44 +2857,44 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>86</v>
       </c>
       <c r="B3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>87</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" t="s">
         <v>94</v>
       </c>
-      <c r="B6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Training video projects set-up. (more:)
1. Scripts almost done. Double-check, record and add to projects.
2. Projects may need adjustent before rendering.

TODO:
1. Second case (manufacturer).
2. Fine configutations and testing of instrument.
</commit_message>
<xml_diff>
--- a/Material/Config/config.xlsx
+++ b/Material/Config/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\0. ProtonDrive\Other computers\DESKTOP-PR117J6\Academic\Projects\2022 - RL Generation\iRL - Experiment with Humans\Material\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B661C37-E23A-4D88-A096-79C4839B3A98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E5D2F3-3836-4E35-90E5-639864276A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
@@ -181,12 +181,6 @@
     <t>Heater On ___________ Minimize Running Time</t>
   </si>
   <si>
-    <t>Maintain Ideal Temperature (previous level)</t>
-  </si>
-  <si>
-    <t>Maintain Ideal Temperature (previous level) ___________ Maintain Ideal Temperature (current level)</t>
-  </si>
-  <si>
     <t>Heater On ___________ Maintain Ideal Temperature (current level)</t>
   </si>
   <si>
@@ -436,15 +430,6 @@
     <t>Signal Heater On __________ On Signal Succeeded, On Signal Failed</t>
   </si>
   <si>
-    <t>Controller</t>
-  </si>
-  <si>
-    <t>Temperature Controlled</t>
-  </si>
-  <si>
-    <t>Controller __________ Temperature Controlled</t>
-  </si>
-  <si>
     <t>On Signal Succeeded</t>
   </si>
   <si>
@@ -686,6 +671,21 @@
   </si>
   <si>
     <t>Satisfaction of the origin affects the satisfaction of the destination (in an unknown or complicated way)</t>
+  </si>
+  <si>
+    <t>Temperature Controller</t>
+  </si>
+  <si>
+    <t>Have Temperature Controlled</t>
+  </si>
+  <si>
+    <t>Maintain Ideal Temperature in the previous stage</t>
+  </si>
+  <si>
+    <t>Maintain Ideal Temperature in the previous stage ___________ Maintain Ideal Temperature (current stage)</t>
+  </si>
+  <si>
+    <t>Controller __________ Have Temperature Controlled</t>
   </si>
 </sst>
 </file>
@@ -1088,8 +1088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:G15"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1125,10 +1125,10 @@
         <v>26</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1151,7 +1151,7 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>129</v>
+        <v>208</v>
       </c>
       <c r="H2" t="s">
         <v>18</v>
@@ -1181,7 +1181,7 @@
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>130</v>
+        <v>209</v>
       </c>
       <c r="H3" t="s">
         <v>19</v>
@@ -1211,7 +1211,7 @@
         <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H4" t="s">
         <v>20</v>
@@ -1241,7 +1241,7 @@
         <v>4</v>
       </c>
       <c r="G5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H5" t="s">
         <v>20</v>
@@ -1271,10 +1271,10 @@
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="H6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I6" t="str">
         <f t="shared" si="0"/>
@@ -1301,10 +1301,10 @@
         <v>6</v>
       </c>
       <c r="G7" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="H7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" si="0"/>
@@ -1331,10 +1331,10 @@
         <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="H8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I8" t="str">
         <f t="shared" si="0"/>
@@ -1361,10 +1361,10 @@
         <v>8</v>
       </c>
       <c r="G9" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="H9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I9" t="str">
         <f t="shared" si="0"/>
@@ -1394,7 +1394,7 @@
         <v>31</v>
       </c>
       <c r="H10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I10" t="str">
         <f t="shared" si="0"/>
@@ -1421,7 +1421,7 @@
         <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="H11" t="s">
         <v>15</v>
@@ -1451,7 +1451,7 @@
         <v>11</v>
       </c>
       <c r="G12" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="H12" t="s">
         <v>16</v>
@@ -1481,7 +1481,7 @@
         <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="H13" t="s">
         <v>16</v>
@@ -1541,7 +1541,7 @@
         <v>14</v>
       </c>
       <c r="G15" t="s">
-        <v>44</v>
+        <v>210</v>
       </c>
       <c r="H15" t="s">
         <v>17</v>
@@ -1571,7 +1571,7 @@
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="H16" t="s">
         <v>13</v>
@@ -1625,10 +1625,10 @@
         <v>2</v>
       </c>
       <c r="G18" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I18" t="str">
         <f t="shared" si="0"/>
@@ -1652,7 +1652,7 @@
         <v>36</v>
       </c>
       <c r="H19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I19" t="str">
         <f t="shared" si="0"/>
@@ -1679,10 +1679,10 @@
         <v>3</v>
       </c>
       <c r="G20" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="H20" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I20" t="str">
         <f t="shared" si="0"/>
@@ -1706,7 +1706,7 @@
         <v>37</v>
       </c>
       <c r="H21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I21" t="str">
         <f t="shared" si="0"/>
@@ -1736,7 +1736,7 @@
         <v>38</v>
       </c>
       <c r="H22" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I22" t="str">
         <f t="shared" si="0"/>
@@ -1766,7 +1766,7 @@
         <v>39</v>
       </c>
       <c r="H23" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I23" t="str">
         <f t="shared" si="0"/>
@@ -1796,7 +1796,7 @@
         <v>40</v>
       </c>
       <c r="H24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I24" t="str">
         <f t="shared" si="0"/>
@@ -1826,7 +1826,7 @@
         <v>41</v>
       </c>
       <c r="H25" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I25" t="str">
         <f t="shared" si="0"/>
@@ -1856,7 +1856,7 @@
         <v>42</v>
       </c>
       <c r="H26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I26" t="str">
         <f t="shared" si="0"/>
@@ -1886,7 +1886,7 @@
         <v>43</v>
       </c>
       <c r="H27" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I27" t="str">
         <f t="shared" si="0"/>
@@ -1913,7 +1913,7 @@
         <v>10</v>
       </c>
       <c r="G28" t="s">
-        <v>45</v>
+        <v>211</v>
       </c>
       <c r="H28" t="s">
         <v>14</v>
@@ -1943,7 +1943,7 @@
         <v>11</v>
       </c>
       <c r="G29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H29" t="s">
         <v>14</v>
@@ -1973,7 +1973,7 @@
         <v>12</v>
       </c>
       <c r="G30" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H30" t="s">
         <v>14</v>
@@ -2003,7 +2003,7 @@
         <v>13</v>
       </c>
       <c r="G31" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H31" t="s">
         <v>14</v>
@@ -2033,10 +2033,10 @@
         <v>14</v>
       </c>
       <c r="G32" t="s">
-        <v>131</v>
+        <v>212</v>
       </c>
       <c r="H32" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="I32" t="str">
         <f t="shared" ref="I32:I58" si="1">VLOOKUP(H32,iRL,2,FALSE)</f>
@@ -2045,10 +2045,10 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B33" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -2063,7 +2063,7 @@
         <v>1</v>
       </c>
       <c r="G33" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="H33" t="s">
         <v>19</v>
@@ -2075,10 +2075,10 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B34" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C34">
         <v>2</v>
@@ -2093,7 +2093,7 @@
         <v>2</v>
       </c>
       <c r="G34" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="H34" t="s">
         <v>19</v>
@@ -2105,10 +2105,10 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B35" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C35">
         <v>3</v>
@@ -2123,7 +2123,7 @@
         <v>3</v>
       </c>
       <c r="G35" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="H35" t="s">
         <v>20</v>
@@ -2135,10 +2135,10 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B36" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C36">
         <v>4</v>
@@ -2153,7 +2153,7 @@
         <v>4</v>
       </c>
       <c r="G36" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="H36" t="s">
         <v>19</v>
@@ -2165,10 +2165,10 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B37" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C37">
         <v>5</v>
@@ -2183,7 +2183,7 @@
         <v>5</v>
       </c>
       <c r="G37" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="H37" t="s">
         <v>20</v>
@@ -2195,10 +2195,10 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B38" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C38">
         <v>6</v>
@@ -2213,7 +2213,7 @@
         <v>6</v>
       </c>
       <c r="G38" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="H38" t="s">
         <v>20</v>
@@ -2225,10 +2225,10 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B39" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C39">
         <v>7</v>
@@ -2243,10 +2243,10 @@
         <v>7</v>
       </c>
       <c r="G39" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="H39" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I39" t="str">
         <f t="shared" si="1"/>
@@ -2255,10 +2255,10 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B40" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C40">
         <v>8</v>
@@ -2273,10 +2273,10 @@
         <v>8</v>
       </c>
       <c r="G40" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="H40" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I40" t="str">
         <f t="shared" si="1"/>
@@ -2285,10 +2285,10 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B41" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C41">
         <v>9</v>
@@ -2303,10 +2303,10 @@
         <v>9</v>
       </c>
       <c r="G41" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="H41" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I41" t="str">
         <f t="shared" si="1"/>
@@ -2315,10 +2315,10 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B42" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C42">
         <v>10</v>
@@ -2333,10 +2333,10 @@
         <v>10</v>
       </c>
       <c r="G42" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="H42" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I42" t="str">
         <f t="shared" si="1"/>
@@ -2345,10 +2345,10 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B43" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C43">
         <v>11</v>
@@ -2363,10 +2363,10 @@
         <v>11</v>
       </c>
       <c r="G43" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="H43" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I43" t="str">
         <f t="shared" si="1"/>
@@ -2375,10 +2375,10 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B44" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C44">
         <v>12</v>
@@ -2393,7 +2393,7 @@
         <v>12</v>
       </c>
       <c r="G44" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="H44" t="s">
         <v>15</v>
@@ -2405,10 +2405,10 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B45" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C45">
         <v>13</v>
@@ -2423,7 +2423,7 @@
         <v>13</v>
       </c>
       <c r="G45" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="H45" t="s">
         <v>16</v>
@@ -2435,10 +2435,10 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B46" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C46">
         <v>14</v>
@@ -2453,7 +2453,7 @@
         <v>14</v>
       </c>
       <c r="G46" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="H46" t="s">
         <v>17</v>
@@ -2465,10 +2465,10 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B47" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C47">
         <v>15</v>
@@ -2483,10 +2483,10 @@
         <v>15</v>
       </c>
       <c r="G47" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="H47" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I47" t="str">
         <f t="shared" si="1"/>
@@ -2495,10 +2495,10 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B48" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C48">
         <v>16</v>
@@ -2513,10 +2513,10 @@
         <v>16</v>
       </c>
       <c r="G48" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="H48" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I48" t="str">
         <f t="shared" si="1"/>
@@ -2525,10 +2525,10 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B49" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -2543,7 +2543,7 @@
         <v>1</v>
       </c>
       <c r="G49" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="H49" t="s">
         <v>12</v>
@@ -2555,10 +2555,10 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B50" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C50">
         <v>2</v>
@@ -2573,7 +2573,7 @@
         <v>2</v>
       </c>
       <c r="G50" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="H50" t="s">
         <v>13</v>
@@ -2585,10 +2585,10 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B51" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C51">
         <v>3</v>
@@ -2603,10 +2603,10 @@
         <v>3</v>
       </c>
       <c r="G51" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="H51" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I51" t="str">
         <f t="shared" si="1"/>
@@ -2615,10 +2615,10 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B52" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C52">
         <v>4</v>
@@ -2633,10 +2633,10 @@
         <v>4</v>
       </c>
       <c r="G52" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="H52" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I52" t="str">
         <f t="shared" si="1"/>
@@ -2645,10 +2645,10 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B53" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C53">
         <v>5</v>
@@ -2663,10 +2663,10 @@
         <v>5</v>
       </c>
       <c r="G53" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="H53" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I53" t="str">
         <f t="shared" si="1"/>
@@ -2675,10 +2675,10 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B54" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C54">
         <v>6</v>
@@ -2693,10 +2693,10 @@
         <v>6</v>
       </c>
       <c r="G54" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="H54" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I54" t="str">
         <f t="shared" si="1"/>
@@ -2705,10 +2705,10 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B55" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C55">
         <v>7</v>
@@ -2723,10 +2723,10 @@
         <v>7</v>
       </c>
       <c r="G55" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="H55" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I55" t="str">
         <f t="shared" si="1"/>
@@ -2735,10 +2735,10 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B56" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C56">
         <v>8</v>
@@ -2753,7 +2753,7 @@
         <v>8</v>
       </c>
       <c r="G56" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="H56" t="s">
         <v>14</v>
@@ -2765,10 +2765,10 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B57" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C57">
         <v>9</v>
@@ -2783,10 +2783,10 @@
         <v>9</v>
       </c>
       <c r="G57" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="H57" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I57" t="str">
         <f t="shared" si="1"/>
@@ -2795,10 +2795,10 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B58" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C58">
         <v>10</v>
@@ -2813,10 +2813,10 @@
         <v>10</v>
       </c>
       <c r="G58" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="H58" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I58" t="str">
         <f t="shared" si="1"/>
@@ -2849,28 +2849,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2887,10 +2887,10 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="F2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G2" t="b">
         <v>0</v>
@@ -2913,10 +2913,10 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F3" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="G3" t="b">
         <v>0</v>
@@ -2939,10 +2939,10 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G4" t="b">
         <v>0</v>
@@ -2953,11 +2953,11 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s">
         <v>54</v>
       </c>
-      <c r="B5" t="s">
-        <v>56</v>
-      </c>
       <c r="C5" t="s">
         <v>27</v>
       </c>
@@ -2965,10 +2965,10 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G5" t="b">
         <v>0</v>
@@ -2979,11 +2979,11 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" t="s">
         <v>55</v>
       </c>
-      <c r="B6" t="s">
-        <v>57</v>
-      </c>
       <c r="C6" t="s">
         <v>27</v>
       </c>
@@ -2991,10 +2991,10 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G6" t="b">
         <v>0</v>
@@ -3005,10 +3005,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C7" t="s">
         <v>27</v>
@@ -3017,10 +3017,10 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F7" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="G7" t="b">
         <v>0</v>
@@ -3034,7 +3034,7 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C8" t="s">
         <v>27</v>
@@ -3043,10 +3043,10 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F8" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="G8" t="b">
         <v>0</v>
@@ -3069,10 +3069,10 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G9" t="b">
         <v>0</v>
@@ -3086,7 +3086,7 @@
         <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C10" t="s">
         <v>27</v>
@@ -3095,10 +3095,10 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="F10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G10" t="b">
         <v>0</v>
@@ -3109,10 +3109,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B11" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
@@ -3121,10 +3121,10 @@
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F11" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="G11" t="b">
         <v>1</v>
@@ -3138,7 +3138,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
@@ -3147,10 +3147,10 @@
         <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F12" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="G12" t="b">
         <v>1</v>
@@ -3164,7 +3164,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="C13" t="s">
         <v>9</v>
@@ -3173,10 +3173,10 @@
         <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F13" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="G13" t="b">
         <v>1</v>
@@ -3187,10 +3187,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C14" t="s">
         <v>9</v>
@@ -3199,10 +3199,10 @@
         <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F14" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="G14" t="b">
         <v>1</v>
@@ -3213,10 +3213,10 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B15" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
@@ -3225,10 +3225,10 @@
         <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="F15" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="G15" t="b">
         <v>1</v>
@@ -3239,10 +3239,10 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B16" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C16" t="s">
         <v>9</v>
@@ -3251,10 +3251,10 @@
         <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="F16" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="G16" t="b">
         <v>1</v>
@@ -3265,10 +3265,10 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B17" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C17" t="s">
         <v>9</v>
@@ -3277,10 +3277,10 @@
         <v>2</v>
       </c>
       <c r="E17" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="F17" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="G17" t="b">
         <v>1</v>
@@ -3294,7 +3294,7 @@
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C18" t="s">
         <v>9</v>
@@ -3303,10 +3303,10 @@
         <v>2</v>
       </c>
       <c r="E18" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="F18" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="G18" t="b">
         <v>1</v>
@@ -3317,10 +3317,10 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>9</v>
@@ -3329,10 +3329,10 @@
         <v>2</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="F19" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="G19" t="b">
         <v>1</v>
@@ -3366,7 +3366,7 @@
         <v>0</v>
       </c>
       <c r="H20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -3394,7 +3394,7 @@
         <v>0</v>
       </c>
       <c r="H21" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -3422,7 +3422,7 @@
         <v>0</v>
       </c>
       <c r="H22" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -3450,7 +3450,7 @@
         <v>0</v>
       </c>
       <c r="H23" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -3478,7 +3478,7 @@
         <v>0</v>
       </c>
       <c r="H24" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -3506,7 +3506,7 @@
         <v>0</v>
       </c>
       <c r="H25" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -3534,7 +3534,7 @@
         <v>0</v>
       </c>
       <c r="H26" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -3562,7 +3562,7 @@
         <v>0</v>
       </c>
       <c r="H27" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -3590,12 +3590,12 @@
         <v>0</v>
       </c>
       <c r="H28" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
@@ -3618,12 +3618,12 @@
         <v>0</v>
       </c>
       <c r="H29" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B30" t="s">
         <v>11</v>
@@ -3646,7 +3646,7 @@
         <v>0</v>
       </c>
       <c r="H30" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -3692,43 +3692,43 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -3736,63 +3736,63 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E2" t="s">
-        <v>65</v>
-      </c>
       <c r="F2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="I2" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="J2" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="K2" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="L2" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="M2" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" t="s">
         <v>67</v>
       </c>
-      <c r="F3" t="s">
-        <v>69</v>
-      </c>
       <c r="G3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -3828,19 +3828,19 @@
         <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="154.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3851,33 +3851,33 @@
         <v>30</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B3" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -3901,71 +3901,71 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" t="s">
         <v>72</v>
-      </c>
-      <c r="B3" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B9" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Training videos complete (draft). Ethics response.
</commit_message>
<xml_diff>
--- a/Material/Config/config.xlsx
+++ b/Material/Config/config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\0. ProtonDrive\Other computers\DESKTOP-PR117J6\Academic\Projects\2022 - RL Generation\iRL - Experiment with Humans\Material\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dropbox\Private\Others\Academic\Projects\2022 - RL Generation\iRL - Experiment with Humans\Material\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E5D2F3-3836-4E35-90E5-639864276A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92508EE5-5E1F-4488-91F6-F9EB13BF4DA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25252" yWindow="-118" windowWidth="25370" windowHeight="13667" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
@@ -253,9 +253,6 @@
     <t>-9jfFPtJNG8</t>
   </si>
   <si>
-    <t>xvJWxwtL6JQ</t>
-  </si>
-  <si>
     <t>intro</t>
   </si>
   <si>
@@ -265,15 +262,6 @@
     <t>completeness</t>
   </si>
   <si>
-    <t>ZyIINfeDCA0</t>
-  </si>
-  <si>
-    <t>ztqen6Dg41o</t>
-  </si>
-  <si>
-    <t>1XIvCNK6Ir4</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -686,6 +674,18 @@
   </si>
   <si>
     <t>Controller __________ Have Temperature Controlled</t>
+  </si>
+  <si>
+    <t>tq5Jlj5PIp4</t>
+  </si>
+  <si>
+    <t>N0nm7sLNOlw</t>
+  </si>
+  <si>
+    <t>D-kUoP-498U</t>
+  </si>
+  <si>
+    <t>HpN6hz41nvI</t>
   </si>
 </sst>
 </file>
@@ -1046,7 +1046,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="350" row="4">
+  <wetp:taskpane dockstate="right" visibility="0" width="401" row="7">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
   <wetp:taskpane dockstate="right" visibility="0" width="350" row="5">
@@ -1067,6 +1067,13 @@
   </we:properties>
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_JIRA_JQL</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
 </we:webextension>
 </file>
 
@@ -1088,21 +1095,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="92.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="92.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="38.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -1125,13 +1132,13 @@
         <v>26</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -1151,7 +1158,7 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="H2" t="s">
         <v>18</v>
@@ -1161,7 +1168,7 @@
         <v>Actor</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -1181,7 +1188,7 @@
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="H3" t="s">
         <v>19</v>
@@ -1191,7 +1198,7 @@
         <v>Goal</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -1211,7 +1218,7 @@
         <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="H4" t="s">
         <v>20</v>
@@ -1221,7 +1228,7 @@
         <v>Task</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -1241,7 +1248,7 @@
         <v>4</v>
       </c>
       <c r="G5" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="H5" t="s">
         <v>20</v>
@@ -1251,7 +1258,7 @@
         <v>Task</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -1271,7 +1278,7 @@
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="H6" t="s">
         <v>52</v>
@@ -1281,7 +1288,7 @@
         <v>Effect (task satisfying)</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1301,7 +1308,7 @@
         <v>6</v>
       </c>
       <c r="G7" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="H7" t="s">
         <v>52</v>
@@ -1311,7 +1318,7 @@
         <v>Effect (task satisfying)</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -1331,7 +1338,7 @@
         <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="H8" t="s">
         <v>52</v>
@@ -1341,7 +1348,7 @@
         <v>Effect (task satisfying)</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -1361,7 +1368,7 @@
         <v>8</v>
       </c>
       <c r="G9" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="H9" t="s">
         <v>52</v>
@@ -1371,7 +1378,7 @@
         <v>Effect (task satisfying)</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -1401,7 +1408,7 @@
         <v>Effect (indirect)</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1421,7 +1428,7 @@
         <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="H11" t="s">
         <v>15</v>
@@ -1431,7 +1438,7 @@
         <v>Pre-Effect</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1451,7 +1458,7 @@
         <v>11</v>
       </c>
       <c r="G12" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="H12" t="s">
         <v>16</v>
@@ -1461,7 +1468,7 @@
         <v>Quality</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -1481,7 +1488,7 @@
         <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="H13" t="s">
         <v>16</v>
@@ -1491,7 +1498,7 @@
         <v>Quality</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -1521,7 +1528,7 @@
         <v>Quality</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1541,7 +1548,7 @@
         <v>14</v>
       </c>
       <c r="G15" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="H15" t="s">
         <v>17</v>
@@ -1551,7 +1558,7 @@
         <v>Pre-Quality</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -1571,7 +1578,7 @@
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="H16" t="s">
         <v>13</v>
@@ -1581,7 +1588,7 @@
         <v>is OR-refined to</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -1605,7 +1612,7 @@
         <v>is OR-refined to</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -1625,7 +1632,7 @@
         <v>2</v>
       </c>
       <c r="G18" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="H18" t="s">
         <v>51</v>
@@ -1635,7 +1642,7 @@
         <v>affects (non-deterministically)</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -1659,7 +1666,7 @@
         <v>affects (non-deterministically)</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -1679,7 +1686,7 @@
         <v>3</v>
       </c>
       <c r="G20" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="H20" t="s">
         <v>51</v>
@@ -1689,7 +1696,7 @@
         <v>affects (non-deterministically)</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -1713,7 +1720,7 @@
         <v>affects (non-deterministically)</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -1743,7 +1750,7 @@
         <v>Effect (indirect)</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -1773,7 +1780,7 @@
         <v>affects (deterministically)</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1803,7 +1810,7 @@
         <v>affects (deterministically)</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -1833,7 +1840,7 @@
         <v>affects (deterministically)</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -1863,7 +1870,7 @@
         <v>affects (deterministically)</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -1893,7 +1900,7 @@
         <v>negatively contributes to</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -1913,7 +1920,7 @@
         <v>10</v>
       </c>
       <c r="G28" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H28" t="s">
         <v>14</v>
@@ -1923,7 +1930,7 @@
         <v>contributes to</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -1953,7 +1960,7 @@
         <v>contributes to</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1983,7 +1990,7 @@
         <v>contributes to</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -2013,7 +2020,7 @@
         <v>contributes to</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -2033,22 +2040,22 @@
         <v>14</v>
       </c>
       <c r="G32" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="H32" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="I32" t="str">
         <f t="shared" ref="I32:I58" si="1">VLOOKUP(H32,iRL,2,FALSE)</f>
         <v>wants to</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B33" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -2063,7 +2070,7 @@
         <v>1</v>
       </c>
       <c r="G33" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="H33" t="s">
         <v>19</v>
@@ -2073,12 +2080,12 @@
         <v>Goal</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B34" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C34">
         <v>2</v>
@@ -2093,7 +2100,7 @@
         <v>2</v>
       </c>
       <c r="G34" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="H34" t="s">
         <v>19</v>
@@ -2103,12 +2110,12 @@
         <v>Goal</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B35" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C35">
         <v>3</v>
@@ -2123,7 +2130,7 @@
         <v>3</v>
       </c>
       <c r="G35" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="H35" t="s">
         <v>20</v>
@@ -2133,12 +2140,12 @@
         <v>Task</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B36" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C36">
         <v>4</v>
@@ -2153,7 +2160,7 @@
         <v>4</v>
       </c>
       <c r="G36" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="H36" t="s">
         <v>19</v>
@@ -2163,12 +2170,12 @@
         <v>Goal</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B37" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C37">
         <v>5</v>
@@ -2183,7 +2190,7 @@
         <v>5</v>
       </c>
       <c r="G37" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="H37" t="s">
         <v>20</v>
@@ -2193,12 +2200,12 @@
         <v>Task</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B38" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C38">
         <v>6</v>
@@ -2213,7 +2220,7 @@
         <v>6</v>
       </c>
       <c r="G38" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="H38" t="s">
         <v>20</v>
@@ -2223,12 +2230,12 @@
         <v>Task</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B39" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C39">
         <v>7</v>
@@ -2243,7 +2250,7 @@
         <v>7</v>
       </c>
       <c r="G39" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="H39" t="s">
         <v>52</v>
@@ -2253,12 +2260,12 @@
         <v>Effect (task satisfying)</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B40" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C40">
         <v>8</v>
@@ -2273,7 +2280,7 @@
         <v>8</v>
       </c>
       <c r="G40" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="H40" t="s">
         <v>52</v>
@@ -2283,12 +2290,12 @@
         <v>Effect (task satisfying)</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B41" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C41">
         <v>9</v>
@@ -2303,7 +2310,7 @@
         <v>9</v>
       </c>
       <c r="G41" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="H41" t="s">
         <v>53</v>
@@ -2313,12 +2320,12 @@
         <v>Effect (task non-satisfying)</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B42" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C42">
         <v>10</v>
@@ -2333,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="G42" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="H42" t="s">
         <v>49</v>
@@ -2343,12 +2350,12 @@
         <v>Effect (indirect)</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B43" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C43">
         <v>11</v>
@@ -2363,7 +2370,7 @@
         <v>11</v>
       </c>
       <c r="G43" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="H43" t="s">
         <v>49</v>
@@ -2373,12 +2380,12 @@
         <v>Effect (indirect)</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B44" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C44">
         <v>12</v>
@@ -2393,7 +2400,7 @@
         <v>12</v>
       </c>
       <c r="G44" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H44" t="s">
         <v>15</v>
@@ -2403,12 +2410,12 @@
         <v>Pre-Effect</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B45" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C45">
         <v>13</v>
@@ -2423,7 +2430,7 @@
         <v>13</v>
       </c>
       <c r="G45" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="H45" t="s">
         <v>16</v>
@@ -2433,12 +2440,12 @@
         <v>Quality</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B46" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C46">
         <v>14</v>
@@ -2453,7 +2460,7 @@
         <v>14</v>
       </c>
       <c r="G46" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="H46" t="s">
         <v>17</v>
@@ -2463,12 +2470,12 @@
         <v>Pre-Quality</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B47" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C47">
         <v>15</v>
@@ -2483,7 +2490,7 @@
         <v>15</v>
       </c>
       <c r="G47" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="H47" t="s">
         <v>52</v>
@@ -2493,12 +2500,12 @@
         <v>Effect (task satisfying)</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B48" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C48">
         <v>16</v>
@@ -2513,7 +2520,7 @@
         <v>16</v>
       </c>
       <c r="G48" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="H48" t="s">
         <v>52</v>
@@ -2523,12 +2530,12 @@
         <v>Effect (task satisfying)</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B49" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -2543,7 +2550,7 @@
         <v>1</v>
       </c>
       <c r="G49" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="H49" t="s">
         <v>12</v>
@@ -2553,12 +2560,12 @@
         <v>is AND-refined to</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B50" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C50">
         <v>2</v>
@@ -2573,7 +2580,7 @@
         <v>2</v>
       </c>
       <c r="G50" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="H50" t="s">
         <v>13</v>
@@ -2583,12 +2590,12 @@
         <v>is OR-refined to</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B51" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C51">
         <v>3</v>
@@ -2603,7 +2610,7 @@
         <v>3</v>
       </c>
       <c r="G51" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="H51" t="s">
         <v>51</v>
@@ -2613,12 +2620,12 @@
         <v>affects (non-deterministically)</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B52" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C52">
         <v>4</v>
@@ -2633,7 +2640,7 @@
         <v>4</v>
       </c>
       <c r="G52" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="H52" t="s">
         <v>50</v>
@@ -2643,12 +2650,12 @@
         <v>affects (deterministically)</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B53" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C53">
         <v>5</v>
@@ -2663,7 +2670,7 @@
         <v>5</v>
       </c>
       <c r="G53" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="H53" t="s">
         <v>50</v>
@@ -2673,12 +2680,12 @@
         <v>affects (deterministically)</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B54" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C54">
         <v>6</v>
@@ -2693,7 +2700,7 @@
         <v>6</v>
       </c>
       <c r="G54" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="H54" t="s">
         <v>50</v>
@@ -2703,12 +2710,12 @@
         <v>affects (deterministically)</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B55" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C55">
         <v>7</v>
@@ -2723,7 +2730,7 @@
         <v>7</v>
       </c>
       <c r="G55" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="H55" t="s">
         <v>50</v>
@@ -2733,12 +2740,12 @@
         <v>affects (deterministically)</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B56" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C56">
         <v>8</v>
@@ -2753,7 +2760,7 @@
         <v>8</v>
       </c>
       <c r="G56" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="H56" t="s">
         <v>14</v>
@@ -2763,12 +2770,12 @@
         <v>contributes to</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B57" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C57">
         <v>9</v>
@@ -2783,7 +2790,7 @@
         <v>9</v>
       </c>
       <c r="G57" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="H57" t="s">
         <v>58</v>
@@ -2793,12 +2800,12 @@
         <v>negatively contributes to</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B58" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C58">
         <v>10</v>
@@ -2813,7 +2820,7 @@
         <v>10</v>
       </c>
       <c r="G58" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="H58" t="s">
         <v>57</v>
@@ -2837,43 +2844,43 @@
       <selection activeCell="H19" sqref="A1:H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="38.85546875" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="68.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" customWidth="1"/>
+    <col min="2" max="2" width="38.88671875" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" customWidth="1"/>
+    <col min="5" max="5" width="68.6640625" customWidth="1"/>
     <col min="6" max="7" width="61" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -2887,10 +2894,10 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="F2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G2" t="b">
         <v>0</v>
@@ -2899,7 +2906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -2913,10 +2920,10 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F3" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="G3" t="b">
         <v>0</v>
@@ -2925,7 +2932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -2939,10 +2946,10 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G4" t="b">
         <v>0</v>
@@ -2951,7 +2958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -2965,10 +2972,10 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G5" t="b">
         <v>0</v>
@@ -2977,7 +2984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -2991,10 +2998,10 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F6" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G6" t="b">
         <v>0</v>
@@ -3003,7 +3010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -3017,10 +3024,10 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F7" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="G7" t="b">
         <v>0</v>
@@ -3029,12 +3036,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C8" t="s">
         <v>27</v>
@@ -3043,10 +3050,10 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F8" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="G8" t="b">
         <v>0</v>
@@ -3055,7 +3062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -3069,10 +3076,10 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F9" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G9" t="b">
         <v>0</v>
@@ -3081,12 +3088,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C10" t="s">
         <v>27</v>
@@ -3095,10 +3102,10 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="F10" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="G10" t="b">
         <v>0</v>
@@ -3107,12 +3114,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B11" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
@@ -3121,10 +3128,10 @@
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F11" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="G11" t="b">
         <v>1</v>
@@ -3133,12 +3140,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
@@ -3147,10 +3154,10 @@
         <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="F12" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="G12" t="b">
         <v>1</v>
@@ -3159,12 +3166,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C13" t="s">
         <v>9</v>
@@ -3173,10 +3180,10 @@
         <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="F13" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="G13" t="b">
         <v>1</v>
@@ -3185,12 +3192,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C14" t="s">
         <v>9</v>
@@ -3199,10 +3206,10 @@
         <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F14" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="G14" t="b">
         <v>1</v>
@@ -3211,12 +3218,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>50</v>
       </c>
       <c r="B15" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
@@ -3225,10 +3232,10 @@
         <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="F15" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="G15" t="b">
         <v>1</v>
@@ -3237,12 +3244,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>57</v>
       </c>
       <c r="B16" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C16" t="s">
         <v>9</v>
@@ -3251,10 +3258,10 @@
         <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F16" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G16" t="b">
         <v>1</v>
@@ -3263,12 +3270,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>58</v>
       </c>
       <c r="B17" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C17" t="s">
         <v>9</v>
@@ -3277,10 +3284,10 @@
         <v>2</v>
       </c>
       <c r="E17" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="F17" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="G17" t="b">
         <v>1</v>
@@ -3289,12 +3296,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C18" t="s">
         <v>9</v>
@@ -3303,10 +3310,10 @@
         <v>2</v>
       </c>
       <c r="E18" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="F18" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="G18" t="b">
         <v>1</v>
@@ -3315,12 +3322,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>9</v>
@@ -3329,10 +3336,10 @@
         <v>2</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="F19" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="G19" t="b">
         <v>1</v>
@@ -3341,7 +3348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -3369,7 +3376,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -3397,7 +3404,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -3425,7 +3432,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -3453,7 +3460,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -3481,7 +3488,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -3509,7 +3516,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -3537,7 +3544,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -3565,7 +3572,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -3593,7 +3600,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>50</v>
       </c>
@@ -3621,7 +3628,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>51</v>
       </c>
@@ -3673,24 +3680,24 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="54.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="63.7109375" customWidth="1"/>
-    <col min="5" max="5" width="36.28515625" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.6640625" customWidth="1"/>
+    <col min="5" max="5" width="36.33203125" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
     <col min="7" max="7" width="41" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.5703125" customWidth="1"/>
-    <col min="9" max="9" width="34.28515625" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.5546875" customWidth="1"/>
+    <col min="9" max="9" width="34.33203125" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>59</v>
       </c>
@@ -3698,40 +3705,40 @@
         <v>60</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3739,7 +3746,7 @@
         <v>61</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>62</v>
@@ -3751,28 +3758,28 @@
         <v>66</v>
       </c>
       <c r="G2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="H2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="I2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="J2" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="K2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="L2" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="M2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>47</v>
       </c>
@@ -3780,7 +3787,7 @@
         <v>61</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>64</v>
@@ -3792,7 +3799,7 @@
         <v>67</v>
       </c>
       <c r="G3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -3815,35 +3822,35 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="128.7109375" customWidth="1"/>
+    <col min="3" max="3" width="128.6640625" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="69.140625" customWidth="1"/>
-    <col min="6" max="6" width="66.7109375" customWidth="1"/>
+    <col min="5" max="5" width="69.109375" customWidth="1"/>
+    <col min="6" max="6" width="66.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" t="s">
         <v>79</v>
       </c>
-      <c r="F1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" ht="154.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" s="3" customFormat="1" ht="154.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>29</v>
       </c>
@@ -3851,33 +3858,33 @@
         <v>30</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="60.25" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -3889,83 +3896,83 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9276482A-FDB8-4250-9ACB-F74FE92B070A}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>69</v>
       </c>
-      <c r="B2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>70</v>
       </c>
-      <c r="B3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B7" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B9" t="b">
         <v>0</v>

</xml_diff>